<commit_message>
Maj Apogée janvier 2019
</commit_message>
<xml_diff>
--- a/data-raw/Composante.xlsx
+++ b/data-raw/Composante.xlsx
@@ -406,9 +406,6 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E42"/>
-  <sheetViews>
-    <sheetView rightToLeft="0" workbookViewId="0"/>
-  </sheetViews>
   <cols>
     <col min="1" max="1" width="21.1051986666667" customWidth="1"/>
     <col min="2" max="5" width="10.7163133333333" customWidth="1"/>
@@ -984,9 +981,6 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView rightToLeft="0" workbookViewId="0"/>
-  </sheetViews>
   <cols>
     <col min="1" max="1" width="25.8129" customWidth="1"/>
     <col min="2" max="3" width="10.7163133333333" customWidth="1"/>
@@ -1064,9 +1058,6 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView rightToLeft="0" workbookViewId="0"/>
-  </sheetViews>
   <cols>
     <col min="1" max="1" width="23.8165" customWidth="1"/>
     <col min="2" max="2" width="10.7163133333333" customWidth="1"/>

</xml_diff>

<commit_message>
Apogée : mise à jour juin 2019
</commit_message>
<xml_diff>
--- a/data-raw/Composante.xlsx
+++ b/data-raw/Composante.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="124">
   <si>
     <t>Composante (code)</t>
   </si>
@@ -45,6 +45,9 @@
     <t>AL3</t>
   </si>
   <si>
+    <t>ALB</t>
+  </si>
+  <si>
     <t>APS</t>
   </si>
   <si>
@@ -66,6 +69,12 @@
     <t>32013</t>
   </si>
   <si>
+    <t>BIO</t>
+  </si>
+  <si>
+    <t>FSI BIOGEO</t>
+  </si>
+  <si>
     <t>CAS</t>
   </si>
   <si>
@@ -75,6 +84,12 @@
     <t>81065</t>
   </si>
   <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>FSI CHIMIE</t>
+  </si>
+  <si>
     <t>DEN</t>
   </si>
   <si>
@@ -87,12 +102,24 @@
     <t>DEUG</t>
   </si>
   <si>
+    <t>EEA</t>
+  </si>
+  <si>
+    <t>FSI EEA</t>
+  </si>
+  <si>
     <t>FCA</t>
   </si>
   <si>
     <t>FSI</t>
   </si>
   <si>
+    <t>INF</t>
+  </si>
+  <si>
+    <t>FSI INFO</t>
+  </si>
+  <si>
     <t>IU1</t>
   </si>
   <si>
@@ -207,9 +234,39 @@
     <t>LANG.VIV.</t>
   </si>
   <si>
+    <t>LVG</t>
+  </si>
+  <si>
+    <t>FSI Langue</t>
+  </si>
+  <si>
+    <t>MAT</t>
+  </si>
+  <si>
+    <t>FSI MATHS</t>
+  </si>
+  <si>
+    <t>MEC</t>
+  </si>
+  <si>
+    <t>FSI MECA</t>
+  </si>
+  <si>
     <t>MIG</t>
   </si>
   <si>
+    <t>MPS</t>
+  </si>
+  <si>
+    <t>Reg.CMP</t>
+  </si>
+  <si>
+    <t>OMP</t>
+  </si>
+  <si>
+    <t>INS</t>
+  </si>
+  <si>
     <t>PCA</t>
   </si>
   <si>
@@ -219,6 +276,18 @@
     <t>PHARMACIE</t>
   </si>
   <si>
+    <t>PHY</t>
+  </si>
+  <si>
+    <t>FSI PHYSIQ</t>
+  </si>
+  <si>
+    <t>PRE</t>
+  </si>
+  <si>
+    <t>PRESIDENCE</t>
+  </si>
+  <si>
     <t>PUR</t>
   </si>
   <si>
@@ -240,12 +309,21 @@
     <t>12202</t>
   </si>
   <si>
+    <t>SCA</t>
+  </si>
+  <si>
+    <t>SCUAPS</t>
+  </si>
+  <si>
     <t>SCU</t>
   </si>
   <si>
     <t>scol.centr</t>
   </si>
   <si>
+    <t>SHN</t>
+  </si>
+  <si>
     <t>STA</t>
   </si>
   <si>
@@ -261,6 +339,15 @@
     <t>IUT TARBES</t>
   </si>
   <si>
+    <t>UTT</t>
+  </si>
+  <si>
+    <t>ComUE</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
     <t>Composante - Commune (lib.)</t>
   </si>
   <si>
@@ -276,7 +363,13 @@
     <t>Composante - Type (lib.)</t>
   </si>
   <si>
+    <t>Coummunauté d'universités/établissements</t>
+  </si>
+  <si>
     <t>Département</t>
+  </si>
+  <si>
+    <t>Institut</t>
   </si>
   <si>
     <t>Institut Universitaire Professionnel</t>
@@ -296,7 +389,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -307,14 +400,8 @@
       <color rgb="00333333"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="00FFFFFF"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,18 +419,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0B64A0"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF8FBFC"/>
+        <fgColor rgb="FFF7F7F7"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -353,31 +434,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="003877A6"/>
+        <color rgb="00DDDDDD"/>
       </left>
       <right style="thin">
-        <color rgb="003877A6"/>
+        <color rgb="00DDDDDD"/>
       </right>
       <top style="thin">
-        <color rgb="003877A6"/>
+        <color rgb="00DDDDDD"/>
       </top>
       <bottom style="thin">
-        <color rgb="00A5A5B1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00EBEBEB"/>
-      </left>
-      <right style="thin">
-        <color rgb="00EBEBEB"/>
-      </right>
-      <top style="thin">
-        <color rgb="00EBEBEB"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="00EBEBEB"/>
+        <color rgb="00DDDDDD"/>
       </bottom>
       <diagonal/>
     </border>
@@ -385,18 +451,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -405,14 +468,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E57"/>
   <cols>
-    <col min="1" max="1" width="21.1051986666667" customWidth="1"/>
+    <col min="1" max="1" width="1.0008" customWidth="1"/>
     <col min="2" max="5" width="10.7163133333333" customWidth="1"/>
     <col min="6" max="6" width="4.67767866666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="26.1317" customHeight="1"/>
+    <row r="1" s="1" customFormat="1" ht="58.663" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -442,16 +505,16 @@
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -470,127 +533,129 @@
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>14</v>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
+    </row>
+    <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>7</v>
+      <c r="E10" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4" t="s">
-        <v>14</v>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>29</v>
+      <c r="D14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -598,335 +663,333 @@
         <v>32</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>29</v>
+      <c r="C16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>29</v>
+      <c r="D18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>29</v>
+      <c r="D20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B22" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>29</v>
+      <c r="D22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B24" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B24" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>29</v>
+      <c r="D24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B26" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>29</v>
+      <c r="D26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="E27" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>29</v>
+      <c r="D28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B29" s="3" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B30" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>61</v>
+      <c r="C30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B31" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B32" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>14</v>
+      <c r="B32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B33" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B34" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>14</v>
+      <c r="B34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B35" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="36" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B36" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>14</v>
+      <c r="C36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B37" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>14</v>
+      <c r="D38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -937,24 +1000,24 @@
         <v>79</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>14</v>
+      <c r="D40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="41" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -964,14 +1027,214 @@
       <c r="C41" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B42" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B43" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B44" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B45" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B46" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B47" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B48" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B49" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B50" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B51" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B52" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B53" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B54" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B55" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B56" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
@@ -982,50 +1245,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
   <cols>
-    <col min="1" max="1" width="25.8129" customWidth="1"/>
+    <col min="1" max="1" width="37.6467986666667" customWidth="1"/>
     <col min="2" max="3" width="10.7163133333333" customWidth="1"/>
     <col min="4" max="4" width="4.67767866666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="5.333" customHeight="1"/>
+    <row r="1" s="1" customFormat="1" ht="51.1968" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>84</v>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>86</v>
+      <c r="B6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -1037,11 +1300,11 @@
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>19</v>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="11.1993" customHeight="1">
@@ -1057,64 +1320,79 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <cols>
-    <col min="1" max="1" width="23.8165" customWidth="1"/>
-    <col min="2" max="2" width="10.7163133333333" customWidth="1"/>
-    <col min="3" max="3" width="42.6397" customWidth="1"/>
+    <col min="1" max="1" width="29.3759986666667" customWidth="1"/>
+    <col min="2" max="3" width="10.7163133333333" customWidth="1"/>
     <col min="4" max="4" width="4.67767866666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="5.333" customHeight="1"/>
+    <row r="1" s="1" customFormat="1" ht="61.3295" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>89</v>
+      <c r="C4" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>91</v>
+      <c r="B6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>